<commit_message>
Migrazione a JustETF: ISIN come identificatore primario, analisi Close-only
- Sostituisce yfinance con JustETF come fonte dati primaria
- ISIN come identificatore univoco (risolve 91 ticker duplicati)
- Analisi tecnica solo Close: MACD e Bollinger Band Width sostituiscono ADX e Volume Ratio
- Corregge 15 ISIN sbagliati (Ossiam/Amundi ticker collision, fuzzy match errati)
- Nuovi file: isin_resolver.py, justetf_fetcher.py, migrate_to_isin.py, fix_duplicate_isins.py
- Database: aggiunta colonna ISIN con indice, nuovo metodo save_close_bulk/get_close_by_isin
- Dashboard: aggiornata con MACD, BB Width, tooltip ISIN, fonte JustETF

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/etf_monitoraggio.xlsx
+++ b/etf_monitoraggio.xlsx
@@ -17,13 +17,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <color rgb="00006600"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00CC0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +56,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N189"/>
+  <dimension ref="A1:O189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,12 +487,12 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ADX</t>
+          <t>MACD Hist</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Vol Ratio</t>
+          <t>BB Width</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
@@ -490,6 +503,11 @@
       <c r="N1" t="inlineStr">
         <is>
           <t>Ultima Modifica</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ISIN</t>
         </is>
       </c>
     </row>
@@ -517,15 +535,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>LU1900066975</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -551,15 +565,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>LU1900067601</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -585,15 +595,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>LU1834983550</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -619,15 +625,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>FR0010405431</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -653,15 +655,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>LU1900066207</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -687,15 +685,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="O7" s="2" t="inlineStr">
+        <is>
+          <t>LU1834983634</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -721,15 +715,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="O8" s="2" t="inlineStr">
+        <is>
+          <t>LU1681046006</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -755,15 +745,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="O9" s="2" t="inlineStr">
+        <is>
+          <t>FR0010524777</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -789,15 +775,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="O10" s="2" t="inlineStr">
+        <is>
+          <t>FR0010524777</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -823,15 +805,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="O11" s="2" t="inlineStr">
+        <is>
+          <t>LU1834988278</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -857,15 +835,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="O12" s="2" t="inlineStr">
+        <is>
+          <t>LU1900066462</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -891,15 +865,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
+          <t>LU1834988609</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -925,15 +895,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>LU2009202107</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -959,15 +925,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="O15" s="2" t="inlineStr">
+        <is>
+          <t>LU1834988864</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -993,15 +955,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+      <c r="O16" s="2" t="inlineStr">
+        <is>
+          <t>FR0010245514</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1027,15 +985,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+      <c r="O17" s="2" t="inlineStr">
+        <is>
+          <t>LU1681037864</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1061,15 +1015,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="O18" s="2" t="inlineStr">
+        <is>
+          <t>LU1287022708</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1095,15 +1045,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+      <c r="O19" s="2" t="inlineStr">
+        <is>
+          <t>LU1737652583</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1129,15 +1075,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="O20" s="2" t="inlineStr">
+        <is>
+          <t>LU1437017350</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1163,15 +1105,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
+      <c r="O21" s="2" t="inlineStr">
+        <is>
+          <t>LU1681045370</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1197,15 +1135,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="O22" s="2" t="inlineStr">
+        <is>
+          <t>LU1681037609</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1231,15 +1165,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+      <c r="O23" s="2" t="inlineStr">
+        <is>
+          <t>LU1834983477</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1265,15 +1195,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
+      <c r="O24" s="2" t="inlineStr">
+        <is>
+          <t>IE000OVF8Q66</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1299,15 +1225,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
+      <c r="O25" s="2" t="inlineStr">
+        <is>
+          <t>LU2469335371</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1333,15 +1255,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
+      <c r="O26" s="2" t="inlineStr">
+        <is>
+          <t>LU1602144732</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1367,15 +1285,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
+      <c r="O27" s="2" t="inlineStr">
+        <is>
+          <t>LU1900068328</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1401,15 +1315,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
+      <c r="O28" s="2" t="inlineStr">
+        <is>
+          <t>LU1829218749</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1435,15 +1345,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
+      <c r="O29" s="2" t="inlineStr">
+        <is>
+          <t>IE00B466KX20</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1469,15 +1375,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
+      <c r="O30" s="2" t="inlineStr">
+        <is>
+          <t>LU0496786905</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1503,15 +1405,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
+      <c r="O31" s="2" t="inlineStr">
+        <is>
+          <t>LU1681042518</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1537,15 +1435,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
+      <c r="O32" s="2" t="inlineStr">
+        <is>
+          <t>LU1829219390</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1571,15 +1465,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
+      <c r="O33" s="2" t="inlineStr">
+        <is>
+          <t>LU1812092168</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1605,15 +1495,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
+      <c r="O34" s="2" t="inlineStr">
+        <is>
+          <t>LU1900068161</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1639,15 +1525,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
+      <c r="O35" s="2" t="inlineStr">
+        <is>
+          <t>IE000D5R9C23</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1673,15 +1555,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
+      <c r="O36" s="2" t="inlineStr">
+        <is>
+          <t>FR0014002CH1</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1707,15 +1585,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
+      <c r="O37" s="2" t="inlineStr">
+        <is>
+          <t>FR0010527275</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1741,15 +1615,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
+      <c r="O38" s="2" t="inlineStr">
+        <is>
+          <t>LU1834987890</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1775,15 +1645,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
+      <c r="O39" s="2" t="inlineStr">
+        <is>
+          <t>LU1834985845</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1809,15 +1675,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
+      <c r="O40" s="2" t="inlineStr">
+        <is>
+          <t>LU1861138961</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1843,15 +1705,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
+      <c r="O41" s="2" t="inlineStr">
+        <is>
+          <t>LU2109787551</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1877,15 +1735,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
+      <c r="O42" s="2" t="inlineStr">
+        <is>
+          <t>LU1681039480</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1911,15 +1765,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
+      <c r="O43" s="2" t="inlineStr">
+        <is>
+          <t>LU1681044647</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1945,15 +1795,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
+      <c r="O44" s="2" t="inlineStr">
+        <is>
+          <t>LU1598689153</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1979,15 +1825,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+      <c r="O45" s="2" t="inlineStr">
+        <is>
+          <t>LU1598690169</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2013,15 +1855,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+      <c r="O46" s="2" t="inlineStr">
+        <is>
+          <t>FR0010261198</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2047,15 +1885,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
+      <c r="O47" s="2" t="inlineStr">
+        <is>
+          <t>LU1437015735</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2081,15 +1915,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+      <c r="O48" s="2" t="inlineStr">
+        <is>
+          <t>FR0010010827</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2115,15 +1945,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
+      <c r="O49" s="2" t="inlineStr">
+        <is>
+          <t>LU2130768844</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2149,15 +1975,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
+      <c r="O50" s="2" t="inlineStr">
+        <is>
+          <t>LU1681042609</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2183,15 +2005,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
+      <c r="O51" s="2" t="inlineStr">
+        <is>
+          <t>LU1681038672</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2217,15 +2035,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
+      <c r="O52" s="2" t="inlineStr">
+        <is>
+          <t>FR0010010827</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2251,15 +2065,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
+      <c r="O53" s="2" t="inlineStr">
+        <is>
+          <t>LU2037748345</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2285,15 +2095,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
+      <c r="O54" s="2" t="inlineStr">
+        <is>
+          <t>IE00000EF730</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2319,15 +2125,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
+      <c r="O55" s="2" t="inlineStr">
+        <is>
+          <t>LU1940199984</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2353,15 +2155,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
+      <c r="O56" s="2" t="inlineStr">
+        <is>
+          <t>LU1940199711</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2387,15 +2185,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
+      <c r="O57" s="2" t="inlineStr">
+        <is>
+          <t>LU1834986900</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2421,15 +2215,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
+      <c r="O58" s="2" t="inlineStr">
+        <is>
+          <t>LU0908501132</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2455,15 +2245,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
+      <c r="O59" s="2" t="inlineStr">
+        <is>
+          <t>LU1681041890</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2489,15 +2275,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="inlineStr"/>
-      <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
+      <c r="O60" s="2" t="inlineStr">
+        <is>
+          <t>LU1900066033</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2523,15 +2305,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
-      <c r="K61" t="inlineStr"/>
-      <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
+      <c r="O61" s="2" t="inlineStr">
+        <is>
+          <t>LU1681037518</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2557,15 +2335,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
-      <c r="K62" t="inlineStr"/>
-      <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr"/>
-      <c r="N62" t="inlineStr"/>
+      <c r="O62" s="2" t="inlineStr">
+        <is>
+          <t>IE000LAP5Z18</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2591,15 +2365,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr"/>
-      <c r="L63" t="inlineStr"/>
-      <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
+      <c r="O63" s="2" t="inlineStr">
+        <is>
+          <t>FR0007054358</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2625,15 +2395,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="inlineStr"/>
-      <c r="K64" t="inlineStr"/>
-      <c r="L64" t="inlineStr"/>
-      <c r="M64" t="inlineStr"/>
-      <c r="N64" t="inlineStr"/>
+      <c r="O64" s="2" t="inlineStr">
+        <is>
+          <t>LU2195226068</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2659,15 +2425,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr"/>
-      <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr"/>
-      <c r="N65" t="inlineStr"/>
+      <c r="O65" s="2" t="inlineStr">
+        <is>
+          <t>LU1602144575</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2693,15 +2455,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
-      <c r="K66" t="inlineStr"/>
-      <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr"/>
-      <c r="N66" t="inlineStr"/>
+      <c r="O66" s="2" t="inlineStr">
+        <is>
+          <t>FR0007056841</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2727,15 +2485,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr"/>
-      <c r="L67" t="inlineStr"/>
-      <c r="M67" t="inlineStr"/>
-      <c r="N67" t="inlineStr"/>
+      <c r="O67" s="2" t="inlineStr">
+        <is>
+          <t>LU2109787635</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2761,15 +2515,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
-      <c r="K68" t="inlineStr"/>
-      <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
+      <c r="O68" s="2" t="inlineStr">
+        <is>
+          <t>IE000KJPDY61</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2795,15 +2545,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
-      <c r="L69" t="inlineStr"/>
-      <c r="M69" t="inlineStr"/>
-      <c r="N69" t="inlineStr"/>
+      <c r="O69" s="2" t="inlineStr">
+        <is>
+          <t>LU1598688189</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2829,15 +2575,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr"/>
-      <c r="N70" t="inlineStr"/>
+      <c r="O70" s="2" t="inlineStr">
+        <is>
+          <t>FR0011758085</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2863,15 +2605,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
-      <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr"/>
-      <c r="M71" t="inlineStr"/>
-      <c r="N71" t="inlineStr"/>
+      <c r="O71" s="2" t="inlineStr">
+        <is>
+          <t>LU1681048127</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2897,15 +2635,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
-      <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr"/>
-      <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
+      <c r="O72" s="2" t="inlineStr">
+        <is>
+          <t>LU1861137484</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -2931,15 +2665,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
-      <c r="J73" t="inlineStr"/>
-      <c r="K73" t="inlineStr"/>
-      <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr"/>
+      <c r="O73" s="2" t="inlineStr">
+        <is>
+          <t>LU1832418773</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -2965,15 +2695,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
-      <c r="N74" t="inlineStr"/>
+      <c r="O74" s="2" t="inlineStr">
+        <is>
+          <t>FR0011720911</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -2999,15 +2725,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
-      <c r="J75" t="inlineStr"/>
-      <c r="K75" t="inlineStr"/>
-      <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
-      <c r="N75" t="inlineStr"/>
+      <c r="O75" s="2" t="inlineStr">
+        <is>
+          <t>LU2059756598</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -3033,15 +2755,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr"/>
-      <c r="J76" t="inlineStr"/>
-      <c r="K76" t="inlineStr"/>
-      <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr"/>
-      <c r="N76" t="inlineStr"/>
+      <c r="O76" s="2" t="inlineStr">
+        <is>
+          <t>LU1829220216</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -3067,15 +2785,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
-      <c r="J77" t="inlineStr"/>
-      <c r="K77" t="inlineStr"/>
-      <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
-      <c r="N77" t="inlineStr"/>
+      <c r="O77" s="2" t="inlineStr">
+        <is>
+          <t>IE000XL4IXU1</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -3101,15 +2815,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
-      <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr"/>
-      <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr"/>
-      <c r="N78" t="inlineStr"/>
+      <c r="O78" s="2" t="inlineStr">
+        <is>
+          <t>LU1650491282</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -3135,15 +2845,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
-      <c r="J79" t="inlineStr"/>
-      <c r="K79" t="inlineStr"/>
-      <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr"/>
-      <c r="N79" t="inlineStr"/>
+      <c r="O79" s="2" t="inlineStr">
+        <is>
+          <t>LU2240851688</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -3169,15 +2875,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr"/>
-      <c r="J80" t="inlineStr"/>
-      <c r="K80" t="inlineStr"/>
-      <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr"/>
-      <c r="N80" t="inlineStr"/>
+      <c r="O80" s="2" t="inlineStr">
+        <is>
+          <t>IE000BUIVY49</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3203,15 +2905,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr"/>
-      <c r="J81" t="inlineStr"/>
-      <c r="K81" t="inlineStr"/>
-      <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr"/>
-      <c r="N81" t="inlineStr"/>
+      <c r="O81" s="2" t="inlineStr">
+        <is>
+          <t>IE0007FM00T9</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -3237,15 +2935,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
-      <c r="I82" t="inlineStr"/>
-      <c r="J82" t="inlineStr"/>
-      <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr"/>
-      <c r="N82" t="inlineStr"/>
+      <c r="O82" s="2" t="inlineStr">
+        <is>
+          <t>LU1598691217</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -3271,15 +2965,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr"/>
-      <c r="K83" t="inlineStr"/>
-      <c r="L83" t="inlineStr"/>
-      <c r="M83" t="inlineStr"/>
-      <c r="N83" t="inlineStr"/>
+      <c r="O83" s="2" t="inlineStr">
+        <is>
+          <t>IE000D8XC064</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3305,15 +2995,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
+      <c r="O84" s="2" t="inlineStr">
+        <is>
+          <t>LU0832435464</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3339,15 +3025,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
+      <c r="O85" s="2" t="inlineStr">
+        <is>
+          <t>LU0533033238</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3373,15 +3055,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
-      <c r="I86" t="inlineStr"/>
-      <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr"/>
-      <c r="M86" t="inlineStr"/>
-      <c r="N86" t="inlineStr"/>
+      <c r="O86" s="2" t="inlineStr">
+        <is>
+          <t>LU1650489385</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -3407,15 +3085,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
-      <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
-      <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
-      <c r="N87" t="inlineStr"/>
+      <c r="O87" s="2" t="inlineStr">
+        <is>
+          <t>IE000NHAIBN0</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -3441,15 +3115,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
-      <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
+      <c r="O88" s="2" t="inlineStr">
+        <is>
+          <t>IE00B4L5Y983</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3475,15 +3145,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
-      <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr"/>
-      <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
+      <c r="O89" s="2" t="inlineStr">
+        <is>
+          <t>LU1681039647</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3509,15 +3175,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
-      <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
+      <c r="O90" s="2" t="inlineStr">
+        <is>
+          <t>IE00085PWS28</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -3543,15 +3205,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
+      <c r="O91" s="2" t="inlineStr">
+        <is>
+          <t>FR0011660927</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -3577,15 +3235,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
+      <c r="O92" s="2" t="inlineStr">
+        <is>
+          <t>LU1437018168</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -3611,15 +3265,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
+      <c r="O93" s="2" t="inlineStr">
+        <is>
+          <t>LU1681043912</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -3645,15 +3295,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr"/>
-      <c r="H94" t="inlineStr"/>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
+      <c r="O94" s="2" t="inlineStr">
+        <is>
+          <t>LU0290357259</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -3679,15 +3325,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
+      <c r="O95" s="2" t="inlineStr">
+        <is>
+          <t>FR0013209921</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -3713,15 +3355,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr"/>
-      <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr"/>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr"/>
-      <c r="N96" t="inlineStr"/>
+      <c r="O96" s="2" t="inlineStr">
+        <is>
+          <t>LU1681046774</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -3747,15 +3385,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
+      <c r="O97" s="2" t="inlineStr">
+        <is>
+          <t>LU1829219127</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -3781,15 +3415,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
+      <c r="O98" s="2" t="inlineStr">
+        <is>
+          <t>LU2182388236</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -3815,15 +3445,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr"/>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr"/>
-      <c r="N99" t="inlineStr"/>
+      <c r="O99" s="2" t="inlineStr">
+        <is>
+          <t>LU0290357176</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -3849,15 +3475,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="inlineStr"/>
-      <c r="H100" t="inlineStr"/>
-      <c r="I100" t="inlineStr"/>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr"/>
-      <c r="M100" t="inlineStr"/>
-      <c r="N100" t="inlineStr"/>
+      <c r="O100" s="2" t="inlineStr">
+        <is>
+          <t>LU1681043599</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -3883,15 +3505,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
+      <c r="O101" s="2" t="inlineStr">
+        <is>
+          <t>FR0010315770</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -3917,15 +3535,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr"/>
-      <c r="G102" t="inlineStr"/>
-      <c r="H102" t="inlineStr"/>
-      <c r="I102" t="inlineStr"/>
-      <c r="J102" t="inlineStr"/>
-      <c r="K102" t="inlineStr"/>
-      <c r="L102" t="inlineStr"/>
-      <c r="M102" t="inlineStr"/>
-      <c r="N102" t="inlineStr"/>
+      <c r="O102" s="2" t="inlineStr">
+        <is>
+          <t>LU1681040496</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -3951,15 +3565,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr"/>
-      <c r="H103" t="inlineStr"/>
-      <c r="I103" t="inlineStr"/>
-      <c r="J103" t="inlineStr"/>
-      <c r="K103" t="inlineStr"/>
-      <c r="L103" t="inlineStr"/>
-      <c r="M103" t="inlineStr"/>
-      <c r="N103" t="inlineStr"/>
+      <c r="O103" s="2" t="inlineStr">
+        <is>
+          <t>LU1737653714</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -3985,15 +3595,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
-      <c r="I104" t="inlineStr"/>
-      <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr"/>
-      <c r="L104" t="inlineStr"/>
-      <c r="M104" t="inlineStr"/>
-      <c r="N104" t="inlineStr"/>
+      <c r="O104" s="2" t="inlineStr">
+        <is>
+          <t>LU2356220926</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -4019,15 +3625,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr"/>
-      <c r="L105" t="inlineStr"/>
-      <c r="M105" t="inlineStr"/>
-      <c r="N105" t="inlineStr"/>
+      <c r="O105" s="2" t="inlineStr">
+        <is>
+          <t>FR0014003IY1</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -4053,15 +3655,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr"/>
-      <c r="L106" t="inlineStr"/>
-      <c r="M106" t="inlineStr"/>
-      <c r="N106" t="inlineStr"/>
+      <c r="O106" s="2" t="inlineStr">
+        <is>
+          <t>LU1681046261</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -4087,15 +3685,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
-      <c r="I107" t="inlineStr"/>
-      <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr"/>
-      <c r="L107" t="inlineStr"/>
-      <c r="M107" t="inlineStr"/>
-      <c r="N107" t="inlineStr"/>
+      <c r="O107" s="2" t="inlineStr">
+        <is>
+          <t>LU1681040496</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -4121,15 +3715,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="inlineStr"/>
-      <c r="H108" t="inlineStr"/>
-      <c r="I108" t="inlineStr"/>
-      <c r="J108" t="inlineStr"/>
-      <c r="K108" t="inlineStr"/>
-      <c r="L108" t="inlineStr"/>
-      <c r="M108" t="inlineStr"/>
-      <c r="N108" t="inlineStr"/>
+      <c r="O108" s="2" t="inlineStr">
+        <is>
+          <t>LU1563454310</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -4155,15 +3745,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr"/>
-      <c r="G109" t="inlineStr"/>
-      <c r="H109" t="inlineStr"/>
-      <c r="I109" t="inlineStr"/>
-      <c r="J109" t="inlineStr"/>
-      <c r="K109" t="inlineStr"/>
-      <c r="L109" t="inlineStr"/>
-      <c r="M109" t="inlineStr"/>
-      <c r="N109" t="inlineStr"/>
+      <c r="O109" s="2" t="inlineStr">
+        <is>
+          <t>LU1525418643</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -4189,15 +3775,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr"/>
-      <c r="G110" t="inlineStr"/>
-      <c r="H110" t="inlineStr"/>
-      <c r="I110" t="inlineStr"/>
-      <c r="J110" t="inlineStr"/>
-      <c r="K110" t="inlineStr"/>
-      <c r="L110" t="inlineStr"/>
-      <c r="M110" t="inlineStr"/>
-      <c r="N110" t="inlineStr"/>
+      <c r="O110" s="2" t="inlineStr">
+        <is>
+          <t>LU1829218822</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -4223,15 +3805,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr"/>
-      <c r="J111" t="inlineStr"/>
-      <c r="K111" t="inlineStr"/>
-      <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr"/>
-      <c r="N111" t="inlineStr"/>
+      <c r="O111" s="2" t="inlineStr">
+        <is>
+          <t>LU2099295466</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4257,15 +3835,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr"/>
-      <c r="G112" t="inlineStr"/>
-      <c r="H112" t="inlineStr"/>
-      <c r="I112" t="inlineStr"/>
-      <c r="J112" t="inlineStr"/>
-      <c r="K112" t="inlineStr"/>
-      <c r="L112" t="inlineStr"/>
-      <c r="M112" t="inlineStr"/>
-      <c r="N112" t="inlineStr"/>
+      <c r="O112" s="2" t="inlineStr">
+        <is>
+          <t>LU2023679090</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -4291,15 +3865,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
-      <c r="I113" t="inlineStr"/>
-      <c r="J113" t="inlineStr"/>
-      <c r="K113" t="inlineStr"/>
-      <c r="L113" t="inlineStr"/>
-      <c r="M113" t="inlineStr"/>
-      <c r="N113" t="inlineStr"/>
+      <c r="O113" s="2" t="inlineStr">
+        <is>
+          <t>IE000KXCEXR3</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -4325,15 +3895,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr"/>
-      <c r="G114" t="inlineStr"/>
-      <c r="H114" t="inlineStr"/>
-      <c r="I114" t="inlineStr"/>
-      <c r="J114" t="inlineStr"/>
-      <c r="K114" t="inlineStr"/>
-      <c r="L114" t="inlineStr"/>
-      <c r="M114" t="inlineStr"/>
-      <c r="N114" t="inlineStr"/>
+      <c r="O114" s="2" t="inlineStr">
+        <is>
+          <t>LU1437018598</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -4359,15 +3925,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr"/>
-      <c r="G115" t="inlineStr"/>
-      <c r="H115" t="inlineStr"/>
-      <c r="I115" t="inlineStr"/>
-      <c r="J115" t="inlineStr"/>
-      <c r="K115" t="inlineStr"/>
-      <c r="L115" t="inlineStr"/>
-      <c r="M115" t="inlineStr"/>
-      <c r="N115" t="inlineStr"/>
+      <c r="O115" s="2" t="inlineStr">
+        <is>
+          <t>LU1287023342</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -4393,15 +3955,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr"/>
-      <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr"/>
-      <c r="J116" t="inlineStr"/>
-      <c r="K116" t="inlineStr"/>
-      <c r="L116" t="inlineStr"/>
-      <c r="M116" t="inlineStr"/>
-      <c r="N116" t="inlineStr"/>
+      <c r="O116" s="2" t="inlineStr">
+        <is>
+          <t>LU1650488494</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -4427,15 +3985,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr"/>
-      <c r="G117" t="inlineStr"/>
-      <c r="H117" t="inlineStr"/>
-      <c r="I117" t="inlineStr"/>
-      <c r="J117" t="inlineStr"/>
-      <c r="K117" t="inlineStr"/>
-      <c r="L117" t="inlineStr"/>
-      <c r="M117" t="inlineStr"/>
-      <c r="N117" t="inlineStr"/>
+      <c r="O117" s="2" t="inlineStr">
+        <is>
+          <t>IE000P1IQS65</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -4461,15 +4015,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F118" t="inlineStr"/>
-      <c r="G118" t="inlineStr"/>
-      <c r="H118" t="inlineStr"/>
-      <c r="I118" t="inlineStr"/>
-      <c r="J118" t="inlineStr"/>
-      <c r="K118" t="inlineStr"/>
-      <c r="L118" t="inlineStr"/>
-      <c r="M118" t="inlineStr"/>
-      <c r="N118" t="inlineStr"/>
+      <c r="O118" s="2" t="inlineStr">
+        <is>
+          <t>LU1287023268</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -4495,15 +4045,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr"/>
-      <c r="G119" t="inlineStr"/>
-      <c r="H119" t="inlineStr"/>
-      <c r="I119" t="inlineStr"/>
-      <c r="J119" t="inlineStr"/>
-      <c r="K119" t="inlineStr"/>
-      <c r="L119" t="inlineStr"/>
-      <c r="M119" t="inlineStr"/>
-      <c r="N119" t="inlineStr"/>
+      <c r="O119" s="2" t="inlineStr">
+        <is>
+          <t>LU1598691050</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -4529,15 +4075,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr"/>
-      <c r="G120" t="inlineStr"/>
-      <c r="H120" t="inlineStr"/>
-      <c r="I120" t="inlineStr"/>
-      <c r="J120" t="inlineStr"/>
-      <c r="K120" t="inlineStr"/>
-      <c r="L120" t="inlineStr"/>
-      <c r="M120" t="inlineStr"/>
-      <c r="N120" t="inlineStr"/>
+      <c r="O120" s="2" t="inlineStr">
+        <is>
+          <t>LU1829219713</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -4563,15 +4105,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
-      <c r="H121" t="inlineStr"/>
-      <c r="I121" t="inlineStr"/>
-      <c r="J121" t="inlineStr"/>
-      <c r="K121" t="inlineStr"/>
-      <c r="L121" t="inlineStr"/>
-      <c r="M121" t="inlineStr"/>
-      <c r="N121" t="inlineStr"/>
+      <c r="O121" s="2" t="inlineStr">
+        <is>
+          <t>LU1681046691</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -4597,15 +4135,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr"/>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
-      <c r="I122" t="inlineStr"/>
-      <c r="J122" t="inlineStr"/>
-      <c r="K122" t="inlineStr"/>
-      <c r="L122" t="inlineStr"/>
-      <c r="M122" t="inlineStr"/>
-      <c r="N122" t="inlineStr"/>
+      <c r="O122" s="2" t="inlineStr">
+        <is>
+          <t>LU1681041114</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -4631,15 +4165,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr"/>
-      <c r="G123" t="inlineStr"/>
-      <c r="H123" t="inlineStr"/>
-      <c r="I123" t="inlineStr"/>
-      <c r="J123" t="inlineStr"/>
-      <c r="K123" t="inlineStr"/>
-      <c r="L123" t="inlineStr"/>
-      <c r="M123" t="inlineStr"/>
-      <c r="N123" t="inlineStr"/>
+      <c r="O123" s="2" t="inlineStr">
+        <is>
+          <t>IE000KXCEXR3</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -4665,15 +4195,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
-      <c r="I124" t="inlineStr"/>
-      <c r="J124" t="inlineStr"/>
-      <c r="K124" t="inlineStr"/>
-      <c r="L124" t="inlineStr"/>
-      <c r="M124" t="inlineStr"/>
-      <c r="N124" t="inlineStr"/>
+      <c r="O124" s="2" t="inlineStr">
+        <is>
+          <t>IE00BF5GB717</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -4699,15 +4225,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr"/>
-      <c r="G125" t="inlineStr"/>
-      <c r="H125" t="inlineStr"/>
-      <c r="I125" t="inlineStr"/>
-      <c r="J125" t="inlineStr"/>
-      <c r="K125" t="inlineStr"/>
-      <c r="L125" t="inlineStr"/>
-      <c r="M125" t="inlineStr"/>
-      <c r="N125" t="inlineStr"/>
+      <c r="O125" s="2" t="inlineStr">
+        <is>
+          <t>LU1435356495</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -4733,15 +4255,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr"/>
-      <c r="G126" t="inlineStr"/>
-      <c r="H126" t="inlineStr"/>
-      <c r="I126" t="inlineStr"/>
-      <c r="J126" t="inlineStr"/>
-      <c r="K126" t="inlineStr"/>
-      <c r="L126" t="inlineStr"/>
-      <c r="M126" t="inlineStr"/>
-      <c r="N126" t="inlineStr"/>
+      <c r="O126" s="2" t="inlineStr">
+        <is>
+          <t>LU1681046345</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -4767,15 +4285,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F127" t="inlineStr"/>
-      <c r="G127" t="inlineStr"/>
-      <c r="H127" t="inlineStr"/>
-      <c r="I127" t="inlineStr"/>
-      <c r="J127" t="inlineStr"/>
-      <c r="K127" t="inlineStr"/>
-      <c r="L127" t="inlineStr"/>
-      <c r="M127" t="inlineStr"/>
-      <c r="N127" t="inlineStr"/>
+      <c r="O127" s="2" t="inlineStr">
+        <is>
+          <t>FR0007075494</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -4801,15 +4315,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F128" t="inlineStr"/>
-      <c r="G128" t="inlineStr"/>
-      <c r="H128" t="inlineStr"/>
-      <c r="I128" t="inlineStr"/>
-      <c r="J128" t="inlineStr"/>
-      <c r="K128" t="inlineStr"/>
-      <c r="L128" t="inlineStr"/>
-      <c r="M128" t="inlineStr"/>
-      <c r="N128" t="inlineStr"/>
+      <c r="O128" s="2" t="inlineStr">
+        <is>
+          <t>LU1650487413</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -4835,15 +4345,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr"/>
-      <c r="G129" t="inlineStr"/>
-      <c r="H129" t="inlineStr"/>
-      <c r="I129" t="inlineStr"/>
-      <c r="J129" t="inlineStr"/>
-      <c r="K129" t="inlineStr"/>
-      <c r="L129" t="inlineStr"/>
-      <c r="M129" t="inlineStr"/>
-      <c r="N129" t="inlineStr"/>
+      <c r="O129" s="2" t="inlineStr">
+        <is>
+          <t>LU1563454310</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -4869,15 +4375,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F130" t="inlineStr"/>
-      <c r="G130" t="inlineStr"/>
-      <c r="H130" t="inlineStr"/>
-      <c r="I130" t="inlineStr"/>
-      <c r="J130" t="inlineStr"/>
-      <c r="K130" t="inlineStr"/>
-      <c r="L130" t="inlineStr"/>
-      <c r="M130" t="inlineStr"/>
-      <c r="N130" t="inlineStr"/>
+      <c r="O130" s="2" t="inlineStr">
+        <is>
+          <t>LU1829219556</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -4903,15 +4405,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F131" t="inlineStr"/>
-      <c r="G131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
-      <c r="I131" t="inlineStr"/>
-      <c r="J131" t="inlineStr"/>
-      <c r="K131" t="inlineStr"/>
-      <c r="L131" t="inlineStr"/>
-      <c r="M131" t="inlineStr"/>
-      <c r="N131" t="inlineStr"/>
+      <c r="O131" s="2" t="inlineStr">
+        <is>
+          <t>LU1812090543</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -4937,15 +4435,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F132" t="inlineStr"/>
-      <c r="G132" t="inlineStr"/>
-      <c r="H132" t="inlineStr"/>
-      <c r="I132" t="inlineStr"/>
-      <c r="J132" t="inlineStr"/>
-      <c r="K132" t="inlineStr"/>
-      <c r="L132" t="inlineStr"/>
-      <c r="M132" t="inlineStr"/>
-      <c r="N132" t="inlineStr"/>
+      <c r="O132" s="2" t="inlineStr">
+        <is>
+          <t>LU2037748774</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -4971,15 +4465,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F133" t="inlineStr"/>
-      <c r="G133" t="inlineStr"/>
-      <c r="H133" t="inlineStr"/>
-      <c r="I133" t="inlineStr"/>
-      <c r="J133" t="inlineStr"/>
-      <c r="K133" t="inlineStr"/>
-      <c r="L133" t="inlineStr"/>
-      <c r="M133" t="inlineStr"/>
-      <c r="N133" t="inlineStr"/>
+      <c r="O133" s="2" t="inlineStr">
+        <is>
+          <t>LU2099295466</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -5005,15 +4495,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F134" t="inlineStr"/>
-      <c r="G134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
-      <c r="I134" t="inlineStr"/>
-      <c r="J134" t="inlineStr"/>
-      <c r="K134" t="inlineStr"/>
-      <c r="L134" t="inlineStr"/>
-      <c r="M134" t="inlineStr"/>
-      <c r="N134" t="inlineStr"/>
+      <c r="O134" s="2" t="inlineStr">
+        <is>
+          <t>LU1435356149</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -5039,15 +4525,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr"/>
-      <c r="G135" t="inlineStr"/>
-      <c r="H135" t="inlineStr"/>
-      <c r="I135" t="inlineStr"/>
-      <c r="J135" t="inlineStr"/>
-      <c r="K135" t="inlineStr"/>
-      <c r="L135" t="inlineStr"/>
-      <c r="M135" t="inlineStr"/>
-      <c r="N135" t="inlineStr"/>
+      <c r="O135" s="2" t="inlineStr">
+        <is>
+          <t>LU0533032859</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -5073,15 +4555,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F136" t="inlineStr"/>
-      <c r="G136" t="inlineStr"/>
-      <c r="H136" t="inlineStr"/>
-      <c r="I136" t="inlineStr"/>
-      <c r="J136" t="inlineStr"/>
-      <c r="K136" t="inlineStr"/>
-      <c r="L136" t="inlineStr"/>
-      <c r="M136" t="inlineStr"/>
-      <c r="N136" t="inlineStr"/>
+      <c r="O136" s="2" t="inlineStr">
+        <is>
+          <t>LU2370241684</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -5107,15 +4585,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F137" t="inlineStr"/>
-      <c r="G137" t="inlineStr"/>
-      <c r="H137" t="inlineStr"/>
-      <c r="I137" t="inlineStr"/>
-      <c r="J137" t="inlineStr"/>
-      <c r="K137" t="inlineStr"/>
-      <c r="L137" t="inlineStr"/>
-      <c r="M137" t="inlineStr"/>
-      <c r="N137" t="inlineStr"/>
+      <c r="O137" s="2" t="inlineStr">
+        <is>
+          <t>FR0013380607</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -5141,15 +4615,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr"/>
-      <c r="G138" t="inlineStr"/>
-      <c r="H138" t="inlineStr"/>
-      <c r="I138" t="inlineStr"/>
-      <c r="J138" t="inlineStr"/>
-      <c r="K138" t="inlineStr"/>
-      <c r="L138" t="inlineStr"/>
-      <c r="M138" t="inlineStr"/>
-      <c r="N138" t="inlineStr"/>
+      <c r="O138" s="2" t="inlineStr">
+        <is>
+          <t>IE0001GSQ2O9</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -5175,15 +4645,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F139" t="inlineStr"/>
-      <c r="G139" t="inlineStr"/>
-      <c r="H139" t="inlineStr"/>
-      <c r="I139" t="inlineStr"/>
-      <c r="J139" t="inlineStr"/>
-      <c r="K139" t="inlineStr"/>
-      <c r="L139" t="inlineStr"/>
-      <c r="M139" t="inlineStr"/>
-      <c r="N139" t="inlineStr"/>
+      <c r="O139" s="3" t="inlineStr">
+        <is>
+          <t>LU1681040900</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -5209,15 +4675,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F140" t="inlineStr"/>
-      <c r="G140" t="inlineStr"/>
-      <c r="H140" t="inlineStr"/>
-      <c r="I140" t="inlineStr"/>
-      <c r="J140" t="inlineStr"/>
-      <c r="K140" t="inlineStr"/>
-      <c r="L140" t="inlineStr"/>
-      <c r="M140" t="inlineStr"/>
-      <c r="N140" t="inlineStr"/>
+      <c r="O140" s="2" t="inlineStr">
+        <is>
+          <t>IE000JJPY166</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -5243,15 +4705,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F141" t="inlineStr"/>
-      <c r="G141" t="inlineStr"/>
-      <c r="H141" t="inlineStr"/>
-      <c r="I141" t="inlineStr"/>
-      <c r="J141" t="inlineStr"/>
-      <c r="K141" t="inlineStr"/>
-      <c r="L141" t="inlineStr"/>
-      <c r="M141" t="inlineStr"/>
-      <c r="N141" t="inlineStr"/>
+      <c r="O141" s="2" t="inlineStr">
+        <is>
+          <t>LU1190417599</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -5277,15 +4735,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F142" t="inlineStr"/>
-      <c r="G142" t="inlineStr"/>
-      <c r="H142" t="inlineStr"/>
-      <c r="I142" t="inlineStr"/>
-      <c r="J142" t="inlineStr"/>
-      <c r="K142" t="inlineStr"/>
-      <c r="L142" t="inlineStr"/>
-      <c r="M142" t="inlineStr"/>
-      <c r="N142" t="inlineStr"/>
+      <c r="O142" s="2" t="inlineStr">
+        <is>
+          <t>FR0010754200</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -5311,15 +4765,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F143" t="inlineStr"/>
-      <c r="G143" t="inlineStr"/>
-      <c r="H143" t="inlineStr"/>
-      <c r="I143" t="inlineStr"/>
-      <c r="J143" t="inlineStr"/>
-      <c r="K143" t="inlineStr"/>
-      <c r="L143" t="inlineStr"/>
-      <c r="M143" t="inlineStr"/>
-      <c r="N143" t="inlineStr"/>
+      <c r="O143" s="2" t="inlineStr">
+        <is>
+          <t>FR0010510800</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -5345,15 +4795,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F144" t="inlineStr"/>
-      <c r="G144" t="inlineStr"/>
-      <c r="H144" t="inlineStr"/>
-      <c r="I144" t="inlineStr"/>
-      <c r="J144" t="inlineStr"/>
-      <c r="K144" t="inlineStr"/>
-      <c r="L144" t="inlineStr"/>
-      <c r="M144" t="inlineStr"/>
-      <c r="N144" t="inlineStr"/>
+      <c r="O144" s="2" t="inlineStr">
+        <is>
+          <t>IE00B27YCF74</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -5379,15 +4825,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr"/>
-      <c r="G145" t="inlineStr"/>
-      <c r="H145" t="inlineStr"/>
-      <c r="I145" t="inlineStr"/>
-      <c r="J145" t="inlineStr"/>
-      <c r="K145" t="inlineStr"/>
-      <c r="L145" t="inlineStr"/>
-      <c r="M145" t="inlineStr"/>
-      <c r="N145" t="inlineStr"/>
+      <c r="O145" s="2" t="inlineStr">
+        <is>
+          <t>LU1437024729</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -5413,15 +4855,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F146" t="inlineStr"/>
-      <c r="G146" t="inlineStr"/>
-      <c r="H146" t="inlineStr"/>
-      <c r="I146" t="inlineStr"/>
-      <c r="J146" t="inlineStr"/>
-      <c r="K146" t="inlineStr"/>
-      <c r="L146" t="inlineStr"/>
-      <c r="M146" t="inlineStr"/>
-      <c r="N146" t="inlineStr"/>
+      <c r="O146" s="2" t="inlineStr">
+        <is>
+          <t>LU1525418726</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -5447,15 +4885,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F147" t="inlineStr"/>
-      <c r="G147" t="inlineStr"/>
-      <c r="H147" t="inlineStr"/>
-      <c r="I147" t="inlineStr"/>
-      <c r="J147" t="inlineStr"/>
-      <c r="K147" t="inlineStr"/>
-      <c r="L147" t="inlineStr"/>
-      <c r="M147" t="inlineStr"/>
-      <c r="N147" t="inlineStr"/>
+      <c r="O147" s="2" t="inlineStr">
+        <is>
+          <t>LU0252633754</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -5481,15 +4915,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F148" t="inlineStr"/>
-      <c r="G148" t="inlineStr"/>
-      <c r="H148" t="inlineStr"/>
-      <c r="I148" t="inlineStr"/>
-      <c r="J148" t="inlineStr"/>
-      <c r="K148" t="inlineStr"/>
-      <c r="L148" t="inlineStr"/>
-      <c r="M148" t="inlineStr"/>
-      <c r="N148" t="inlineStr"/>
+      <c r="O148" s="2" t="inlineStr">
+        <is>
+          <t>LU1812091194</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -5515,15 +4945,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr"/>
-      <c r="G149" t="inlineStr"/>
-      <c r="H149" t="inlineStr"/>
-      <c r="I149" t="inlineStr"/>
-      <c r="J149" t="inlineStr"/>
-      <c r="K149" t="inlineStr"/>
-      <c r="L149" t="inlineStr"/>
-      <c r="M149" t="inlineStr"/>
-      <c r="N149" t="inlineStr"/>
+      <c r="O149" s="2" t="inlineStr">
+        <is>
+          <t>LU1900069219</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -5549,15 +4975,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr"/>
-      <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
-      <c r="I150" t="inlineStr"/>
-      <c r="J150" t="inlineStr"/>
-      <c r="K150" t="inlineStr"/>
-      <c r="L150" t="inlineStr"/>
-      <c r="M150" t="inlineStr"/>
-      <c r="N150" t="inlineStr"/>
+      <c r="O150" s="2" t="inlineStr">
+        <is>
+          <t>LU1435356065</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -5583,15 +5005,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F151" t="inlineStr"/>
-      <c r="G151" t="inlineStr"/>
-      <c r="H151" t="inlineStr"/>
-      <c r="I151" t="inlineStr"/>
-      <c r="J151" t="inlineStr"/>
-      <c r="K151" t="inlineStr"/>
-      <c r="L151" t="inlineStr"/>
-      <c r="M151" t="inlineStr"/>
-      <c r="N151" t="inlineStr"/>
+      <c r="O151" s="2" t="inlineStr">
+        <is>
+          <t>LU1686831030</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -5617,15 +5035,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F152" t="inlineStr"/>
-      <c r="G152" t="inlineStr"/>
-      <c r="H152" t="inlineStr"/>
-      <c r="I152" t="inlineStr"/>
-      <c r="J152" t="inlineStr"/>
-      <c r="K152" t="inlineStr"/>
-      <c r="L152" t="inlineStr"/>
-      <c r="M152" t="inlineStr"/>
-      <c r="N152" t="inlineStr"/>
+      <c r="O152" s="2" t="inlineStr">
+        <is>
+          <t>LU1681041205</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -5651,15 +5065,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F153" t="inlineStr"/>
-      <c r="G153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
-      <c r="I153" t="inlineStr"/>
-      <c r="J153" t="inlineStr"/>
-      <c r="K153" t="inlineStr"/>
-      <c r="L153" t="inlineStr"/>
-      <c r="M153" t="inlineStr"/>
-      <c r="N153" t="inlineStr"/>
+      <c r="O153" s="2" t="inlineStr">
+        <is>
+          <t>IE000R7HJVO6</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -5685,15 +5095,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F154" t="inlineStr"/>
-      <c r="G154" t="inlineStr"/>
-      <c r="H154" t="inlineStr"/>
-      <c r="I154" t="inlineStr"/>
-      <c r="J154" t="inlineStr"/>
-      <c r="K154" t="inlineStr"/>
-      <c r="L154" t="inlineStr"/>
-      <c r="M154" t="inlineStr"/>
-      <c r="N154" t="inlineStr"/>
+      <c r="O154" s="2" t="inlineStr">
+        <is>
+          <t>IE00B1FZS798</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -5719,15 +5125,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F155" t="inlineStr"/>
-      <c r="G155" t="inlineStr"/>
-      <c r="H155" t="inlineStr"/>
-      <c r="I155" t="inlineStr"/>
-      <c r="J155" t="inlineStr"/>
-      <c r="K155" t="inlineStr"/>
-      <c r="L155" t="inlineStr"/>
-      <c r="M155" t="inlineStr"/>
-      <c r="N155" t="inlineStr"/>
+      <c r="O155" s="2" t="inlineStr">
+        <is>
+          <t>LU1681049109</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -5753,15 +5155,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F156" t="inlineStr"/>
-      <c r="G156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
-      <c r="I156" t="inlineStr"/>
-      <c r="J156" t="inlineStr"/>
-      <c r="K156" t="inlineStr"/>
-      <c r="L156" t="inlineStr"/>
-      <c r="M156" t="inlineStr"/>
-      <c r="N156" t="inlineStr"/>
+      <c r="O156" s="2" t="inlineStr">
+        <is>
+          <t>LU1686830909</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -5787,15 +5185,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F157" t="inlineStr"/>
-      <c r="G157" t="inlineStr"/>
-      <c r="H157" t="inlineStr"/>
-      <c r="I157" t="inlineStr"/>
-      <c r="J157" t="inlineStr"/>
-      <c r="K157" t="inlineStr"/>
-      <c r="L157" t="inlineStr"/>
-      <c r="M157" t="inlineStr"/>
-      <c r="N157" t="inlineStr"/>
+      <c r="O157" s="2" t="inlineStr">
+        <is>
+          <t>LU1681048804</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -5821,15 +5215,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F158" t="inlineStr"/>
-      <c r="G158" t="inlineStr"/>
-      <c r="H158" t="inlineStr"/>
-      <c r="I158" t="inlineStr"/>
-      <c r="J158" t="inlineStr"/>
-      <c r="K158" t="inlineStr"/>
-      <c r="L158" t="inlineStr"/>
-      <c r="M158" t="inlineStr"/>
-      <c r="N158" t="inlineStr"/>
+      <c r="O158" s="2" t="inlineStr">
+        <is>
+          <t>LU1285960032</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -5855,15 +5245,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F159" t="inlineStr"/>
-      <c r="G159" t="inlineStr"/>
-      <c r="H159" t="inlineStr"/>
-      <c r="I159" t="inlineStr"/>
-      <c r="J159" t="inlineStr"/>
-      <c r="K159" t="inlineStr"/>
-      <c r="L159" t="inlineStr"/>
-      <c r="M159" t="inlineStr"/>
-      <c r="N159" t="inlineStr"/>
+      <c r="O159" s="2" t="inlineStr">
+        <is>
+          <t>LU2089239276</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -5889,15 +5275,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr"/>
-      <c r="G160" t="inlineStr"/>
-      <c r="H160" t="inlineStr"/>
-      <c r="I160" t="inlineStr"/>
-      <c r="J160" t="inlineStr"/>
-      <c r="K160" t="inlineStr"/>
-      <c r="L160" t="inlineStr"/>
-      <c r="M160" t="inlineStr"/>
-      <c r="N160" t="inlineStr"/>
+      <c r="O160" s="2" t="inlineStr">
+        <is>
+          <t>LU1708330235</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -5923,15 +5305,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F161" t="inlineStr"/>
-      <c r="G161" t="inlineStr"/>
-      <c r="H161" t="inlineStr"/>
-      <c r="I161" t="inlineStr"/>
-      <c r="J161" t="inlineStr"/>
-      <c r="K161" t="inlineStr"/>
-      <c r="L161" t="inlineStr"/>
-      <c r="M161" t="inlineStr"/>
-      <c r="N161" t="inlineStr"/>
+      <c r="O161" s="2" t="inlineStr">
+        <is>
+          <t>LU1285959703</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -5957,15 +5335,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F162" t="inlineStr"/>
-      <c r="G162" t="inlineStr"/>
-      <c r="H162" t="inlineStr"/>
-      <c r="I162" t="inlineStr"/>
-      <c r="J162" t="inlineStr"/>
-      <c r="K162" t="inlineStr"/>
-      <c r="L162" t="inlineStr"/>
-      <c r="M162" t="inlineStr"/>
-      <c r="N162" t="inlineStr"/>
+      <c r="O162" s="2" t="inlineStr">
+        <is>
+          <t>LU1437016204</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -5991,15 +5365,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F163" t="inlineStr"/>
-      <c r="G163" t="inlineStr"/>
-      <c r="H163" t="inlineStr"/>
-      <c r="I163" t="inlineStr"/>
-      <c r="J163" t="inlineStr"/>
-      <c r="K163" t="inlineStr"/>
-      <c r="L163" t="inlineStr"/>
-      <c r="M163" t="inlineStr"/>
-      <c r="N163" t="inlineStr"/>
+      <c r="O163" s="2" t="inlineStr">
+        <is>
+          <t>LU1285959885</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -6025,15 +5395,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F164" t="inlineStr"/>
-      <c r="G164" t="inlineStr"/>
-      <c r="H164" t="inlineStr"/>
-      <c r="I164" t="inlineStr"/>
-      <c r="J164" t="inlineStr"/>
-      <c r="K164" t="inlineStr"/>
-      <c r="L164" t="inlineStr"/>
-      <c r="M164" t="inlineStr"/>
-      <c r="N164" t="inlineStr"/>
+      <c r="O164" s="2" t="inlineStr">
+        <is>
+          <t>IE0000U24AJ9</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -6059,15 +5425,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr"/>
-      <c r="G165" t="inlineStr"/>
-      <c r="H165" t="inlineStr"/>
-      <c r="I165" t="inlineStr"/>
-      <c r="J165" t="inlineStr"/>
-      <c r="K165" t="inlineStr"/>
-      <c r="L165" t="inlineStr"/>
-      <c r="M165" t="inlineStr"/>
-      <c r="N165" t="inlineStr"/>
+      <c r="O165" s="2" t="inlineStr">
+        <is>
+          <t>IE000R85HL30</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -6093,15 +5455,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F166" t="inlineStr"/>
-      <c r="G166" t="inlineStr"/>
-      <c r="H166" t="inlineStr"/>
-      <c r="I166" t="inlineStr"/>
-      <c r="J166" t="inlineStr"/>
-      <c r="K166" t="inlineStr"/>
-      <c r="L166" t="inlineStr"/>
-      <c r="M166" t="inlineStr"/>
-      <c r="N166" t="inlineStr"/>
+      <c r="O166" s="2" t="inlineStr">
+        <is>
+          <t>LU1834988518</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -6127,15 +5485,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F167" t="inlineStr"/>
-      <c r="G167" t="inlineStr"/>
-      <c r="H167" t="inlineStr"/>
-      <c r="I167" t="inlineStr"/>
-      <c r="J167" t="inlineStr"/>
-      <c r="K167" t="inlineStr"/>
-      <c r="L167" t="inlineStr"/>
-      <c r="M167" t="inlineStr"/>
-      <c r="N167" t="inlineStr"/>
+      <c r="O167" s="2" t="inlineStr">
+        <is>
+          <t>LU1900067940</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -6161,15 +5515,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr"/>
-      <c r="G168" t="inlineStr"/>
-      <c r="H168" t="inlineStr"/>
-      <c r="I168" t="inlineStr"/>
-      <c r="J168" t="inlineStr"/>
-      <c r="K168" t="inlineStr"/>
-      <c r="L168" t="inlineStr"/>
-      <c r="M168" t="inlineStr"/>
-      <c r="N168" t="inlineStr"/>
+      <c r="O168" s="2" t="inlineStr">
+        <is>
+          <t>LU1900068914</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -6195,15 +5545,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F169" t="inlineStr"/>
-      <c r="G169" t="inlineStr"/>
-      <c r="H169" t="inlineStr"/>
-      <c r="I169" t="inlineStr"/>
-      <c r="J169" t="inlineStr"/>
-      <c r="K169" t="inlineStr"/>
-      <c r="L169" t="inlineStr"/>
-      <c r="M169" t="inlineStr"/>
-      <c r="N169" t="inlineStr"/>
+      <c r="O169" s="2" t="inlineStr">
+        <is>
+          <t>IE0008TKP6O7</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -6229,15 +5575,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F170" t="inlineStr"/>
-      <c r="G170" t="inlineStr"/>
-      <c r="H170" t="inlineStr"/>
-      <c r="I170" t="inlineStr"/>
-      <c r="J170" t="inlineStr"/>
-      <c r="K170" t="inlineStr"/>
-      <c r="L170" t="inlineStr"/>
-      <c r="M170" t="inlineStr"/>
-      <c r="N170" t="inlineStr"/>
+      <c r="O170" s="2" t="inlineStr">
+        <is>
+          <t>IE0009VWHAE6</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -6263,15 +5605,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F171" t="inlineStr"/>
-      <c r="G171" t="inlineStr"/>
-      <c r="H171" t="inlineStr"/>
-      <c r="I171" t="inlineStr"/>
-      <c r="J171" t="inlineStr"/>
-      <c r="K171" t="inlineStr"/>
-      <c r="L171" t="inlineStr"/>
-      <c r="M171" t="inlineStr"/>
-      <c r="N171" t="inlineStr"/>
+      <c r="O171" s="2" t="inlineStr">
+        <is>
+          <t>IE000PEAJOT0</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -6297,15 +5635,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F172" t="inlineStr"/>
-      <c r="G172" t="inlineStr"/>
-      <c r="H172" t="inlineStr"/>
-      <c r="I172" t="inlineStr"/>
-      <c r="J172" t="inlineStr"/>
-      <c r="K172" t="inlineStr"/>
-      <c r="L172" t="inlineStr"/>
-      <c r="M172" t="inlineStr"/>
-      <c r="N172" t="inlineStr"/>
+      <c r="O172" s="2" t="inlineStr">
+        <is>
+          <t>IE000QWCYQT0</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -6331,15 +5665,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F173" t="inlineStr"/>
-      <c r="G173" t="inlineStr"/>
-      <c r="H173" t="inlineStr"/>
-      <c r="I173" t="inlineStr"/>
-      <c r="J173" t="inlineStr"/>
-      <c r="K173" t="inlineStr"/>
-      <c r="L173" t="inlineStr"/>
-      <c r="M173" t="inlineStr"/>
-      <c r="N173" t="inlineStr"/>
+      <c r="O173" s="2" t="inlineStr">
+        <is>
+          <t>FR0010361683</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -6365,15 +5695,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F174" t="inlineStr"/>
-      <c r="G174" t="inlineStr"/>
-      <c r="H174" t="inlineStr"/>
-      <c r="I174" t="inlineStr"/>
-      <c r="J174" t="inlineStr"/>
-      <c r="K174" t="inlineStr"/>
-      <c r="L174" t="inlineStr"/>
-      <c r="M174" t="inlineStr"/>
-      <c r="N174" t="inlineStr"/>
+      <c r="O174" s="2" t="inlineStr">
+        <is>
+          <t>LU1834987973</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -6399,15 +5725,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F175" t="inlineStr"/>
-      <c r="G175" t="inlineStr"/>
-      <c r="H175" t="inlineStr"/>
-      <c r="I175" t="inlineStr"/>
-      <c r="J175" t="inlineStr"/>
-      <c r="K175" t="inlineStr"/>
-      <c r="L175" t="inlineStr"/>
-      <c r="M175" t="inlineStr"/>
-      <c r="N175" t="inlineStr"/>
+      <c r="O175" s="2" t="inlineStr">
+        <is>
+          <t>LU1681043086</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -6433,15 +5755,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F176" t="inlineStr"/>
-      <c r="G176" t="inlineStr"/>
-      <c r="H176" t="inlineStr"/>
-      <c r="I176" t="inlineStr"/>
-      <c r="J176" t="inlineStr"/>
-      <c r="K176" t="inlineStr"/>
-      <c r="L176" t="inlineStr"/>
-      <c r="M176" t="inlineStr"/>
-      <c r="N176" t="inlineStr"/>
+      <c r="O176" s="2" t="inlineStr">
+        <is>
+          <t>LU1681048630</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -6467,15 +5785,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F177" t="inlineStr"/>
-      <c r="G177" t="inlineStr"/>
-      <c r="H177" t="inlineStr"/>
-      <c r="I177" t="inlineStr"/>
-      <c r="J177" t="inlineStr"/>
-      <c r="K177" t="inlineStr"/>
-      <c r="L177" t="inlineStr"/>
-      <c r="M177" t="inlineStr"/>
-      <c r="N177" t="inlineStr"/>
+      <c r="O177" s="2" t="inlineStr">
+        <is>
+          <t>LU1681038599</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -6501,15 +5815,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr"/>
-      <c r="G178" t="inlineStr"/>
-      <c r="H178" t="inlineStr"/>
-      <c r="I178" t="inlineStr"/>
-      <c r="J178" t="inlineStr"/>
-      <c r="K178" t="inlineStr"/>
-      <c r="L178" t="inlineStr"/>
-      <c r="M178" t="inlineStr"/>
-      <c r="N178" t="inlineStr"/>
+      <c r="O178" s="2" t="inlineStr">
+        <is>
+          <t>LU1954152853</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -6535,15 +5845,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr"/>
-      <c r="G179" t="inlineStr"/>
-      <c r="H179" t="inlineStr"/>
-      <c r="I179" t="inlineStr"/>
-      <c r="J179" t="inlineStr"/>
-      <c r="K179" t="inlineStr"/>
-      <c r="L179" t="inlineStr"/>
-      <c r="M179" t="inlineStr"/>
-      <c r="N179" t="inlineStr"/>
+      <c r="O179" s="2" t="inlineStr">
+        <is>
+          <t>LU2023678282</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -6569,15 +5875,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr"/>
-      <c r="G180" t="inlineStr"/>
-      <c r="H180" t="inlineStr"/>
-      <c r="I180" t="inlineStr"/>
-      <c r="J180" t="inlineStr"/>
-      <c r="K180" t="inlineStr"/>
-      <c r="L180" t="inlineStr"/>
-      <c r="M180" t="inlineStr"/>
-      <c r="N180" t="inlineStr"/>
+      <c r="O180" s="2" t="inlineStr">
+        <is>
+          <t>LU1829221024</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -6603,15 +5905,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
-      <c r="I181" t="inlineStr"/>
-      <c r="J181" t="inlineStr"/>
-      <c r="K181" t="inlineStr"/>
-      <c r="L181" t="inlineStr"/>
-      <c r="M181" t="inlineStr"/>
-      <c r="N181" t="inlineStr"/>
+      <c r="O181" s="2" t="inlineStr">
+        <is>
+          <t>LU1681038243</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -6637,15 +5935,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr"/>
-      <c r="G182" t="inlineStr"/>
-      <c r="H182" t="inlineStr"/>
-      <c r="I182" t="inlineStr"/>
-      <c r="J182" t="inlineStr"/>
-      <c r="K182" t="inlineStr"/>
-      <c r="L182" t="inlineStr"/>
-      <c r="M182" t="inlineStr"/>
-      <c r="N182" t="inlineStr"/>
+      <c r="O182" s="2" t="inlineStr">
+        <is>
+          <t>IE000G0E83X3</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -6671,15 +5965,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr"/>
-      <c r="G183" t="inlineStr"/>
-      <c r="H183" t="inlineStr"/>
-      <c r="I183" t="inlineStr"/>
-      <c r="J183" t="inlineStr"/>
-      <c r="K183" t="inlineStr"/>
-      <c r="L183" t="inlineStr"/>
-      <c r="M183" t="inlineStr"/>
-      <c r="N183" t="inlineStr"/>
+      <c r="O183" s="2" t="inlineStr">
+        <is>
+          <t>LU1834988781</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -6705,15 +5995,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F184" t="inlineStr"/>
-      <c r="G184" t="inlineStr"/>
-      <c r="H184" t="inlineStr"/>
-      <c r="I184" t="inlineStr"/>
-      <c r="J184" t="inlineStr"/>
-      <c r="K184" t="inlineStr"/>
-      <c r="L184" t="inlineStr"/>
-      <c r="M184" t="inlineStr"/>
-      <c r="N184" t="inlineStr"/>
+      <c r="O184" s="2" t="inlineStr">
+        <is>
+          <t>LU2023678449</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -6739,15 +6025,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr"/>
-      <c r="G185" t="inlineStr"/>
-      <c r="H185" t="inlineStr"/>
-      <c r="I185" t="inlineStr"/>
-      <c r="J185" t="inlineStr"/>
-      <c r="K185" t="inlineStr"/>
-      <c r="L185" t="inlineStr"/>
-      <c r="M185" t="inlineStr"/>
-      <c r="N185" t="inlineStr"/>
+      <c r="O185" s="2" t="inlineStr">
+        <is>
+          <t>LU1861132840</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -6773,15 +6055,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F186" t="inlineStr"/>
-      <c r="G186" t="inlineStr"/>
-      <c r="H186" t="inlineStr"/>
-      <c r="I186" t="inlineStr"/>
-      <c r="J186" t="inlineStr"/>
-      <c r="K186" t="inlineStr"/>
-      <c r="L186" t="inlineStr"/>
-      <c r="M186" t="inlineStr"/>
-      <c r="N186" t="inlineStr"/>
+      <c r="O186" s="2" t="inlineStr">
+        <is>
+          <t>LU1900065811</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -6807,15 +6085,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F187" t="inlineStr"/>
-      <c r="G187" t="inlineStr"/>
-      <c r="H187" t="inlineStr"/>
-      <c r="I187" t="inlineStr"/>
-      <c r="J187" t="inlineStr"/>
-      <c r="K187" t="inlineStr"/>
-      <c r="L187" t="inlineStr"/>
-      <c r="M187" t="inlineStr"/>
-      <c r="N187" t="inlineStr"/>
+      <c r="O187" s="2" t="inlineStr">
+        <is>
+          <t>LU0533033667</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -6841,15 +6115,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F188" t="inlineStr"/>
-      <c r="G188" t="inlineStr"/>
-      <c r="H188" t="inlineStr"/>
-      <c r="I188" t="inlineStr"/>
-      <c r="J188" t="inlineStr"/>
-      <c r="K188" t="inlineStr"/>
-      <c r="L188" t="inlineStr"/>
-      <c r="M188" t="inlineStr"/>
-      <c r="N188" t="inlineStr"/>
+      <c r="O188" s="2" t="inlineStr">
+        <is>
+          <t>LU2023678878</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -6875,15 +6145,11 @@
           <t>Milano</t>
         </is>
       </c>
-      <c r="F189" t="inlineStr"/>
-      <c r="G189" t="inlineStr"/>
-      <c r="H189" t="inlineStr"/>
-      <c r="I189" t="inlineStr"/>
-      <c r="J189" t="inlineStr"/>
-      <c r="K189" t="inlineStr"/>
-      <c r="L189" t="inlineStr"/>
-      <c r="M189" t="inlineStr"/>
-      <c r="N189" t="inlineStr"/>
+      <c r="O189" s="2" t="inlineStr">
+        <is>
+          <t>LU3038520774</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>